<commit_message>
Add stationery to model and update order schema
Update API of Order to fix with stationery
</commit_message>
<xml_diff>
--- a/server/file.xlsx
+++ b/server/file.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="97">
   <si>
     <t>name</t>
   </si>
@@ -57,28 +57,265 @@
     <t>Hài hước</t>
   </si>
   <si>
-    <t>Tôi thấy hao vàng trên cỏ xanh1</t>
-  </si>
-  <si>
-    <t>Tôi thấy hao vàng trên cỏ xanh2</t>
-  </si>
-  <si>
-    <t>Tôi thấy hao vàng trên cỏ xanh3</t>
-  </si>
-  <si>
-    <t>Tôi thấy hao vàng trên cỏ xanh4</t>
-  </si>
-  <si>
-    <t>Tôi thấy hao vàng trên cỏ xanh5</t>
-  </si>
-  <si>
-    <t>Tôi thấy hao vàng trên cỏ xanh6</t>
-  </si>
-  <si>
-    <t>Tôi thấy hao vàng trên cỏ xanh7</t>
-  </si>
-  <si>
-    <t>Tôi thấy hao vàng trên cỏ xanh8</t>
+    <t>Trinh thám</t>
+  </si>
+  <si>
+    <t>Văn học</t>
+  </si>
+  <si>
+    <t>Nghệ thuật</t>
+  </si>
+  <si>
+    <t>Tiểu thuyết</t>
+  </si>
+  <si>
+    <t>Tâm lý</t>
+  </si>
+  <si>
+    <t>Tâm linh</t>
+  </si>
+  <si>
+    <t>Tôn giáo</t>
+  </si>
+  <si>
+    <t>Sách thiếu nhi</t>
+  </si>
+  <si>
+    <t>Khoa học</t>
+  </si>
+  <si>
+    <t>Công nghệ</t>
+  </si>
+  <si>
+    <t>Chính trị</t>
+  </si>
+  <si>
+    <t>Pháp luật</t>
+  </si>
+  <si>
+    <t>Kinh tế</t>
+  </si>
+  <si>
+    <t>Viễn tưởng</t>
+  </si>
+  <si>
+    <t>Kinh dị</t>
+  </si>
+  <si>
+    <t>Giật gân</t>
+  </si>
+  <si>
+    <t>Truyện ngắn</t>
+  </si>
+  <si>
+    <t>Dạy nấu ăn</t>
+  </si>
+  <si>
+    <t>Lịch sử</t>
+  </si>
+  <si>
+    <t>Truyền cảm hứng</t>
+  </si>
+  <si>
+    <t>Bí ẩn</t>
+  </si>
+  <si>
+    <t>Tình cảm</t>
+  </si>
+  <si>
+    <t>Hồi ký</t>
+  </si>
+  <si>
+    <t>Lập trình</t>
+  </si>
+  <si>
+    <t>Kỹ năng sống</t>
+  </si>
+  <si>
+    <t>Sách giáo khoa</t>
+  </si>
+  <si>
+    <t>Tiếng Nhật</t>
+  </si>
+  <si>
+    <t>Tiếng Anh</t>
+  </si>
+  <si>
+    <t>Tiếng Trung</t>
+  </si>
+  <si>
+    <t>Tiếng Nga</t>
+  </si>
+  <si>
+    <t>Tiếng Đức</t>
+  </si>
+  <si>
+    <t>Tiếng Hàn</t>
+  </si>
+  <si>
+    <t>Tiếng Pháp</t>
+  </si>
+  <si>
+    <t>Các ngôn ngữ khác</t>
+  </si>
+  <si>
+    <t>Tôi thấy hao vàng trên cỏ xanh</t>
+  </si>
+  <si>
+    <t>Bút</t>
+  </si>
+  <si>
+    <t>Giấy</t>
+  </si>
+  <si>
+    <t>Bìa hồ sơ</t>
+  </si>
+  <si>
+    <t>Dụng cụ vẽ</t>
+  </si>
+  <si>
+    <t>Điện tử</t>
+  </si>
+  <si>
+    <t>Làm đẹp</t>
+  </si>
+  <si>
+    <t>Đồ chơi</t>
+  </si>
+  <si>
+    <t>Đồ trang trí</t>
+  </si>
+  <si>
+    <t>Sách tô màu</t>
+  </si>
+  <si>
+    <t>Tượng</t>
+  </si>
+  <si>
+    <t>Đồ thủ công</t>
+  </si>
+  <si>
+    <t>Tranh cát</t>
+  </si>
+  <si>
+    <t>Board game</t>
+  </si>
+  <si>
+    <t>Bút highlight</t>
+  </si>
+  <si>
+    <t>Tôi là Bêtô</t>
+  </si>
+  <si>
+    <t>Cho tôi một xin một vé đi tuổi thơ</t>
+  </si>
+  <si>
+    <t>Không gia đình</t>
+  </si>
+  <si>
+    <t>Hector Malot</t>
+  </si>
+  <si>
+    <t>Số đỏ</t>
+  </si>
+  <si>
+    <t>Vũ Trọng Phụng</t>
+  </si>
+  <si>
+    <t>Tắt đèn</t>
+  </si>
+  <si>
+    <t>Ngô Tất Tố</t>
+  </si>
+  <si>
+    <t>Tình và rác</t>
+  </si>
+  <si>
+    <t>Ivan Klima</t>
+  </si>
+  <si>
+    <t>Thời gian để sống và thời gian để chết</t>
+  </si>
+  <si>
+    <t>Erich Maria Remarque</t>
+  </si>
+  <si>
+    <t>Người dọn dẹp hiện trường án mạng</t>
+  </si>
+  <si>
+    <t>Lư Lạp Lạp</t>
+  </si>
+  <si>
+    <t>Ghi chép pháp y - Những cái chết bí ẩn</t>
+  </si>
+  <si>
+    <t>Lưu Hiểu Huy</t>
+  </si>
+  <si>
+    <t>Harry Porter 1</t>
+  </si>
+  <si>
+    <t>Harry Porter 2</t>
+  </si>
+  <si>
+    <t>Harry Porter 3</t>
+  </si>
+  <si>
+    <t>Harry Porter 4</t>
+  </si>
+  <si>
+    <t>Harry Porter 5</t>
+  </si>
+  <si>
+    <t>Harry Porter 6</t>
+  </si>
+  <si>
+    <t>Harry Porter 7</t>
+  </si>
+  <si>
+    <t>J.K.Rowling</t>
+  </si>
+  <si>
+    <t>Truyện Trạng Quỳnh</t>
+  </si>
+  <si>
+    <t>Tiếu lâm Việt Nam hay nhất</t>
+  </si>
+  <si>
+    <t>1 Nụ cười bằng 10 thang thuốc bổ</t>
+  </si>
+  <si>
+    <t>Đời về cơ bản là buồn cười</t>
+  </si>
+  <si>
+    <t>Lắt léo tiếng Việt</t>
+  </si>
+  <si>
+    <t>Trạng cười Việt Nam</t>
+  </si>
+  <si>
+    <t>Cơ hội đổi đời</t>
+  </si>
+  <si>
+    <t>Mạnh Linh</t>
+  </si>
+  <si>
+    <t>Đức Anh</t>
+  </si>
+  <si>
+    <t>Trần Tường Minh</t>
+  </si>
+  <si>
+    <t>Lê Bích</t>
+  </si>
+  <si>
+    <t>Lê Minh Quốc</t>
+  </si>
+  <si>
+    <t>Nhiều tác giả</t>
+  </si>
+  <si>
+    <t>Minh Phong</t>
   </si>
 </sst>
 </file>
@@ -396,10 +633,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -436,7 +673,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>44</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
@@ -451,183 +688,554 @@
         <v>20000</v>
       </c>
       <c r="F2">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="G2" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>59</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
       </c>
       <c r="C3">
-        <v>2013</v>
+        <v>2018</v>
       </c>
       <c r="D3" t="s">
         <v>8</v>
       </c>
       <c r="E3">
-        <v>20000</v>
+        <v>68000</v>
       </c>
       <c r="F3">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="G3" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>60</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
       </c>
       <c r="C4">
-        <v>2014</v>
+        <v>2018</v>
       </c>
       <c r="D4" t="s">
         <v>8</v>
       </c>
       <c r="E4">
-        <v>20000</v>
+        <v>64000</v>
       </c>
       <c r="F4">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="G4" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5">
+        <v>2021</v>
+      </c>
+      <c r="D5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5">
+        <v>120000</v>
+      </c>
+      <c r="F5">
+        <v>50</v>
+      </c>
+      <c r="G5" t="s">
         <v>13</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5">
-        <v>2015</v>
-      </c>
-      <c r="D5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5">
-        <v>20000</v>
-      </c>
-      <c r="F5">
-        <v>40</v>
-      </c>
-      <c r="G5" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>63</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>64</v>
       </c>
       <c r="C6">
-        <v>2016</v>
+        <v>2021</v>
       </c>
       <c r="D6" t="s">
         <v>8</v>
       </c>
       <c r="E6">
-        <v>20000</v>
+        <v>44000</v>
       </c>
       <c r="F6">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="G6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>65</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>66</v>
       </c>
       <c r="C7">
-        <v>2017</v>
+        <v>2020</v>
       </c>
       <c r="D7" t="s">
         <v>8</v>
       </c>
       <c r="E7">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="F7">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="G7" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>67</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>68</v>
       </c>
       <c r="C8">
-        <v>2018</v>
+        <v>2020</v>
       </c>
       <c r="D8" t="s">
         <v>8</v>
       </c>
       <c r="E8">
-        <v>20000</v>
+        <v>98000</v>
       </c>
       <c r="F8">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="G8" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>69</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
+        <v>70</v>
       </c>
       <c r="C9">
-        <v>2019</v>
+        <v>2012</v>
       </c>
       <c r="D9" t="s">
         <v>8</v>
       </c>
       <c r="E9">
-        <v>20000</v>
+        <v>80000</v>
       </c>
       <c r="F9">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="G9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>71</v>
+      </c>
+      <c r="B10" t="s">
+        <v>72</v>
+      </c>
+      <c r="C10">
+        <v>2023</v>
+      </c>
+      <c r="D10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10">
+        <v>76000</v>
+      </c>
+      <c r="F10">
+        <v>50</v>
+      </c>
+      <c r="G10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>73</v>
+      </c>
+      <c r="B11" t="s">
+        <v>74</v>
+      </c>
+      <c r="C11">
+        <v>2022</v>
+      </c>
+      <c r="D11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11">
+        <v>150000</v>
+      </c>
+      <c r="F11">
+        <v>50</v>
+      </c>
+      <c r="G11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>75</v>
+      </c>
+      <c r="B12" t="s">
+        <v>82</v>
+      </c>
+      <c r="C12">
+        <v>2022</v>
+      </c>
+      <c r="D12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12">
+        <v>120000</v>
+      </c>
+      <c r="F12">
+        <v>50</v>
+      </c>
+      <c r="G12" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>76</v>
+      </c>
+      <c r="B13" t="s">
+        <v>82</v>
+      </c>
+      <c r="C13">
+        <v>2022</v>
+      </c>
+      <c r="D13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13">
+        <v>135000</v>
+      </c>
+      <c r="F13">
+        <v>50</v>
+      </c>
+      <c r="G13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>77</v>
+      </c>
+      <c r="B14" t="s">
+        <v>82</v>
+      </c>
+      <c r="C14">
+        <v>2022</v>
+      </c>
+      <c r="D14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14">
+        <v>149000</v>
+      </c>
+      <c r="F14">
+        <v>50</v>
+      </c>
+      <c r="G14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>78</v>
+      </c>
+      <c r="B15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C15">
+        <v>2022</v>
+      </c>
+      <c r="D15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15">
+        <v>300000</v>
+      </c>
+      <c r="F15">
+        <v>50</v>
+      </c>
+      <c r="G15" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>79</v>
+      </c>
+      <c r="B16" t="s">
+        <v>82</v>
+      </c>
+      <c r="C16">
+        <v>2022</v>
+      </c>
+      <c r="D16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16">
+        <v>248000</v>
+      </c>
+      <c r="F16">
+        <v>50</v>
+      </c>
+      <c r="G16" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>80</v>
+      </c>
+      <c r="B17" t="s">
+        <v>82</v>
+      </c>
+      <c r="C17">
+        <v>2022</v>
+      </c>
+      <c r="D17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17">
+        <v>196000</v>
+      </c>
+      <c r="F17">
+        <v>50</v>
+      </c>
+      <c r="G17" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>81</v>
+      </c>
+      <c r="B18" t="s">
+        <v>82</v>
+      </c>
+      <c r="C18">
+        <v>2022</v>
+      </c>
+      <c r="D18" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18">
+        <v>196000</v>
+      </c>
+      <c r="F18">
+        <v>50</v>
+      </c>
+      <c r="G18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>83</v>
+      </c>
+      <c r="B19" t="s">
+        <v>90</v>
+      </c>
+      <c r="C19">
+        <v>2021</v>
+      </c>
+      <c r="D19" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19">
+        <v>23000</v>
+      </c>
+      <c r="F19">
+        <v>50</v>
+      </c>
+      <c r="G19" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>84</v>
+      </c>
+      <c r="B20" t="s">
+        <v>91</v>
+      </c>
+      <c r="C20">
+        <v>2016</v>
+      </c>
+      <c r="D20" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20">
+        <v>28000</v>
+      </c>
+      <c r="F20">
+        <v>50</v>
+      </c>
+      <c r="G20" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>85</v>
+      </c>
+      <c r="B21" t="s">
+        <v>92</v>
+      </c>
+      <c r="C21">
+        <v>2022</v>
+      </c>
+      <c r="D21" t="s">
+        <v>8</v>
+      </c>
+      <c r="E21">
+        <v>24000</v>
+      </c>
+      <c r="F21">
+        <v>50</v>
+      </c>
+      <c r="G21" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>86</v>
+      </c>
+      <c r="B22" t="s">
+        <v>93</v>
+      </c>
+      <c r="C22">
+        <v>2022</v>
+      </c>
+      <c r="D22" t="s">
+        <v>8</v>
+      </c>
+      <c r="E22">
+        <v>72000</v>
+      </c>
+      <c r="F22">
+        <v>50</v>
+      </c>
+      <c r="G22" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>87</v>
+      </c>
+      <c r="B23" t="s">
+        <v>94</v>
+      </c>
+      <c r="C23">
+        <v>2017</v>
+      </c>
+      <c r="D23" t="s">
+        <v>8</v>
+      </c>
+      <c r="E23">
+        <v>68000</v>
+      </c>
+      <c r="F23">
+        <v>50</v>
+      </c>
+      <c r="G23" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>88</v>
+      </c>
+      <c r="B24" t="s">
+        <v>95</v>
+      </c>
+      <c r="C24">
+        <v>2016</v>
+      </c>
+      <c r="D24" t="s">
+        <v>8</v>
+      </c>
+      <c r="E24">
+        <v>77000</v>
+      </c>
+      <c r="F24">
+        <v>50</v>
+      </c>
+      <c r="G24" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>89</v>
+      </c>
+      <c r="B25" t="s">
+        <v>96</v>
+      </c>
+      <c r="C25">
+        <v>2020</v>
+      </c>
+      <c r="D25" t="s">
+        <v>8</v>
+      </c>
+      <c r="E25">
+        <v>84000</v>
+      </c>
+      <c r="F25">
+        <v>50</v>
+      </c>
+      <c r="G25" t="s">
         <v>9</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A50"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -642,6 +1250,251 @@
         <v>0</v>
       </c>
     </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>58</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>